<commit_message>
Se termina el proceso para OPERARIOS y para RUTAS queda pendiente el proceso para vuelos
</commit_message>
<xml_diff>
--- a/TareasPendientes.xlsx
+++ b/TareasPendientes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s0d0m\Desktop\ControlAereo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B24B282-803C-424C-ACEF-3469628F8951}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05C7A7C0-DF29-4646-BE6F-9E58F5CC3C70}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19800" windowHeight="11760" xr2:uid="{2AA835B2-1F20-4455-9D06-8CE4E3030FC7}"/>
+    <workbookView xWindow="4185" yWindow="0" windowWidth="15375" windowHeight="7995" xr2:uid="{2AA835B2-1F20-4455-9D06-8CE4E3030FC7}"/>
   </bookViews>
   <sheets>
     <sheet name="Backend" sheetId="1" r:id="rId1"/>
@@ -125,7 +125,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -147,6 +147,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -178,12 +184,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -504,7 +511,7 @@
   <dimension ref="B2:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10:D13"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -588,7 +595,7 @@
       <c r="E6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="4"/>
+      <c r="F6" s="5"/>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
@@ -603,7 +610,7 @@
       <c r="E7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="4"/>
+      <c r="F7" s="5"/>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
@@ -621,22 +628,22 @@
       <c r="F8" s="4"/>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="5"/>
+      <c r="D10" s="6"/>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Funcional hasta la fecha, falta la funcion del plus
</commit_message>
<xml_diff>
--- a/TareasPendientes.xlsx
+++ b/TareasPendientes.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s0d0m\Desktop\ControlAereo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05C7A7C0-DF29-4646-BE6F-9E58F5CC3C70}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{151FEB1D-D6B6-4AB9-8F3B-A4DCA9CBF53B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4185" yWindow="0" windowWidth="15375" windowHeight="7995" xr2:uid="{2AA835B2-1F20-4455-9D06-8CE4E3030FC7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19800" windowHeight="11760" xr2:uid="{2AA835B2-1F20-4455-9D06-8CE4E3030FC7}"/>
   </bookViews>
   <sheets>
     <sheet name="Backend" sheetId="1" r:id="rId1"/>
+    <sheet name="Diagramas" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="50">
   <si>
     <t>Tabla</t>
   </si>
@@ -103,6 +104,78 @@
   </si>
   <si>
     <t>./src/rutas/vueloruta.js</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       </t>
+  </si>
+  <si>
+    <t>|</t>
+  </si>
+  <si>
+    <t>Informe 2</t>
+  </si>
+  <si>
+    <t>Informe 1</t>
+  </si>
+  <si>
+    <t>Listar</t>
+  </si>
+  <si>
+    <t>Mostrar Aerolinea</t>
+  </si>
+  <si>
+    <t>FINALIZADO</t>
+  </si>
+  <si>
+    <t>Modificacion Aerolinea</t>
+  </si>
+  <si>
+    <t>SIN INICIAR</t>
+  </si>
+  <si>
+    <t>Creacion Aerolinea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">K </t>
+  </si>
+  <si>
+    <t>Menu Inicio</t>
+  </si>
+  <si>
+    <t>Look Feel</t>
+  </si>
+  <si>
+    <t>Wire Frame</t>
+  </si>
+  <si>
+    <t>Flujo de navegacion</t>
+  </si>
+  <si>
+    <t>Secuencia</t>
+  </si>
+  <si>
+    <t>Actividades</t>
+  </si>
+  <si>
+    <t>WORD</t>
+  </si>
+  <si>
+    <t>Paquetes</t>
+  </si>
+  <si>
+    <t>Contenido estaticos</t>
+  </si>
+  <si>
+    <t>ModeloFisico de la base de datos</t>
+  </si>
+  <si>
+    <t>Modelo de CLASES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diagrama de analisis </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Casos de uso </t>
   </si>
 </sst>
 </file>
@@ -125,7 +198,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -156,8 +229,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="39">
     <border>
       <left/>
       <right/>
@@ -180,20 +265,663 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -511,7 +1239,7 @@
   <dimension ref="B2:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="C10" sqref="C10:D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -595,7 +1323,7 @@
       <c r="E6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="5"/>
+      <c r="F6" s="4"/>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
@@ -610,7 +1338,7 @@
       <c r="E7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="5"/>
+      <c r="F7" s="4"/>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
@@ -628,22 +1356,22 @@
       <c r="F8" s="4"/>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="6"/>
+      <c r="D10" s="5"/>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -651,4 +1379,400 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4310FA1-B41D-42CB-A612-C0A2A75A318D}">
+  <dimension ref="B3:AB15"/>
+  <sheetViews>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="O16" sqref="O16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="25.5703125" customWidth="1"/>
+    <col min="3" max="6" width="8.7109375" customWidth="1"/>
+    <col min="7" max="8" width="7.7109375" customWidth="1"/>
+    <col min="9" max="9" width="20.85546875" customWidth="1"/>
+    <col min="10" max="10" width="9" customWidth="1"/>
+    <col min="11" max="11" width="7.28515625" customWidth="1"/>
+    <col min="12" max="12" width="8" customWidth="1"/>
+    <col min="13" max="25" width="7.5703125" customWidth="1"/>
+    <col min="27" max="27" width="15.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="2:28" ht="45.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="64"/>
+      <c r="C4" s="62" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" s="63"/>
+      <c r="E4" s="62" t="s">
+        <v>48</v>
+      </c>
+      <c r="F4" s="63"/>
+      <c r="G4" s="62" t="s">
+        <v>47</v>
+      </c>
+      <c r="H4" s="61"/>
+      <c r="I4" s="60" t="s">
+        <v>46</v>
+      </c>
+      <c r="J4" s="59" t="s">
+        <v>45</v>
+      </c>
+      <c r="K4" s="58"/>
+      <c r="L4" s="56" t="s">
+        <v>44</v>
+      </c>
+      <c r="M4" s="55"/>
+      <c r="N4" s="56" t="s">
+        <v>43</v>
+      </c>
+      <c r="O4" s="57"/>
+      <c r="P4" s="56" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q4" s="55"/>
+      <c r="R4" s="56" t="s">
+        <v>41</v>
+      </c>
+      <c r="S4" s="55"/>
+      <c r="T4" s="56" t="s">
+        <v>40</v>
+      </c>
+      <c r="U4" s="57"/>
+      <c r="V4" s="56" t="s">
+        <v>39</v>
+      </c>
+      <c r="W4" s="55"/>
+      <c r="X4" s="56" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y4" s="55"/>
+      <c r="Z4" s="54"/>
+    </row>
+    <row r="5" spans="2:28" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="27"/>
+      <c r="E5" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="27"/>
+      <c r="G5" s="52" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="53"/>
+      <c r="I5" s="52" t="s">
+        <v>11</v>
+      </c>
+      <c r="J5" s="52" t="s">
+        <v>11</v>
+      </c>
+      <c r="K5" s="53"/>
+      <c r="L5" s="52" t="s">
+        <v>11</v>
+      </c>
+      <c r="M5" s="51"/>
+      <c r="N5" s="50" t="s">
+        <v>11</v>
+      </c>
+      <c r="O5" s="49"/>
+      <c r="P5" s="48" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q5" s="47"/>
+      <c r="R5" s="46" t="s">
+        <v>11</v>
+      </c>
+      <c r="S5" s="45"/>
+      <c r="T5" s="44" t="s">
+        <v>11</v>
+      </c>
+      <c r="U5" s="43"/>
+      <c r="V5" s="44" t="s">
+        <v>11</v>
+      </c>
+      <c r="W5" s="43"/>
+      <c r="X5" s="42" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y5" s="41"/>
+    </row>
+    <row r="6" spans="2:28" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="27"/>
+      <c r="E6" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="27"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="26"/>
+      <c r="I6" s="25"/>
+      <c r="J6" s="25"/>
+      <c r="K6" s="26"/>
+      <c r="L6" s="25"/>
+      <c r="M6" s="24"/>
+      <c r="N6" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="O6" s="12"/>
+      <c r="P6" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q6" s="9"/>
+      <c r="R6" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="S6" s="39"/>
+      <c r="T6" s="21"/>
+      <c r="U6" s="22"/>
+      <c r="V6" s="21"/>
+      <c r="W6" s="22"/>
+      <c r="X6" s="21"/>
+      <c r="Y6" s="20"/>
+      <c r="AA6" s="35" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB6" s="38"/>
+    </row>
+    <row r="7" spans="2:28" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="27"/>
+      <c r="E7" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="27"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="26"/>
+      <c r="I7" s="25"/>
+      <c r="J7" s="25"/>
+      <c r="K7" s="26"/>
+      <c r="L7" s="25"/>
+      <c r="M7" s="24"/>
+      <c r="N7" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="O7" s="12"/>
+      <c r="P7" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q7" s="11"/>
+      <c r="R7" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="S7" s="36"/>
+      <c r="T7" s="21"/>
+      <c r="U7" s="22"/>
+      <c r="V7" s="21"/>
+      <c r="W7" s="22"/>
+      <c r="X7" s="21"/>
+      <c r="Y7" s="20"/>
+      <c r="AA7" s="35" t="s">
+        <v>32</v>
+      </c>
+      <c r="AB7" s="34"/>
+    </row>
+    <row r="8" spans="2:28" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="27"/>
+      <c r="E8" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="27"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="26"/>
+      <c r="I8" s="25"/>
+      <c r="J8" s="25"/>
+      <c r="K8" s="26"/>
+      <c r="L8" s="25"/>
+      <c r="M8" s="24"/>
+      <c r="N8" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="O8" s="12"/>
+      <c r="P8" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q8" s="11"/>
+      <c r="R8" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="S8" s="32"/>
+      <c r="T8" s="21"/>
+      <c r="U8" s="22"/>
+      <c r="V8" s="21"/>
+      <c r="W8" s="22"/>
+      <c r="X8" s="21"/>
+      <c r="Y8" s="20"/>
+    </row>
+    <row r="9" spans="2:28" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="27"/>
+      <c r="E9" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="27"/>
+      <c r="G9" s="25"/>
+      <c r="H9" s="26"/>
+      <c r="I9" s="25"/>
+      <c r="J9" s="25"/>
+      <c r="K9" s="26"/>
+      <c r="L9" s="25"/>
+      <c r="M9" s="24"/>
+      <c r="N9" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="O9" s="12"/>
+      <c r="P9" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q9" s="11"/>
+      <c r="R9" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="S9" s="30"/>
+      <c r="T9" s="21"/>
+      <c r="U9" s="22"/>
+      <c r="V9" s="21"/>
+      <c r="W9" s="22"/>
+      <c r="X9" s="21"/>
+      <c r="Y9" s="20"/>
+    </row>
+    <row r="10" spans="2:28" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="27"/>
+      <c r="E10" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="27"/>
+      <c r="G10" s="25"/>
+      <c r="H10" s="26"/>
+      <c r="I10" s="25"/>
+      <c r="J10" s="25"/>
+      <c r="K10" s="26"/>
+      <c r="L10" s="25"/>
+      <c r="M10" s="24"/>
+      <c r="N10" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="O10" s="12"/>
+      <c r="P10" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q10" s="11"/>
+      <c r="R10" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="S10" s="23"/>
+      <c r="T10" s="21"/>
+      <c r="U10" s="22"/>
+      <c r="V10" s="21"/>
+      <c r="W10" s="22"/>
+      <c r="X10" s="21"/>
+      <c r="Y10" s="20"/>
+    </row>
+    <row r="11" spans="2:28" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="17"/>
+      <c r="E11" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="17"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="16"/>
+      <c r="L11" s="15"/>
+      <c r="M11" s="14"/>
+      <c r="N11" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="O11" s="12"/>
+      <c r="P11" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q11" s="11"/>
+      <c r="R11" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="S11" s="9"/>
+      <c r="T11" s="7"/>
+      <c r="U11" s="8"/>
+      <c r="V11" s="7"/>
+      <c r="W11" s="8"/>
+      <c r="X11" s="7"/>
+      <c r="Y11" s="6"/>
+    </row>
+    <row r="14" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="E15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="18">
+    <mergeCell ref="G5:H11"/>
+    <mergeCell ref="I5:I11"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="J5:K11"/>
+    <mergeCell ref="L5:M11"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="P4:Q4"/>
+    <mergeCell ref="R4:S4"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="T4:U4"/>
+    <mergeCell ref="T5:U11"/>
+    <mergeCell ref="V4:W4"/>
+    <mergeCell ref="V5:W11"/>
+    <mergeCell ref="X4:Y4"/>
+    <mergeCell ref="X5:Y11"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>